<commit_message>
added support for col/row
</commit_message>
<xml_diff>
--- a/sampledata/sampleTransferccc123.xlsx
+++ b/sampledata/sampleTransferccc123.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>Source Plate Barcode</t>
   </si>
@@ -51,7 +51,10 @@
     <t>ccc123</t>
   </si>
   <si>
-    <t>ssdest000000141jul15</t>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>ssdest000000141jul16</t>
   </si>
 </sst>
 </file>
@@ -128,8 +131,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,7 +188,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -201,6 +206,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -218,6 +224,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,7 +557,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -590,15 +597,15 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -616,7 +623,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -634,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -652,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -669,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -686,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -703,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -720,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>8</v>

</xml_diff>